<commit_message>
Updated variation and parameter storage
</commit_message>
<xml_diff>
--- a/Outputs/RIF/Tables/popPK_CFRs.xlsx
+++ b/Outputs/RIF/Tables/popPK_CFRs.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="405" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="420" uniqueCount="13">
   <si>
     <t>Oral Dose</t>
   </si>
@@ -53,6 +53,15 @@
   </si>
   <si>
     <t>Day 1, n = 100</t>
+  </si>
+  <si>
+    <t>Day 1, n = 1</t>
+  </si>
+  <si>
+    <t>Day 1, n = 10</t>
+  </si>
+  <si>
+    <t>Day 1, n = 1000</t>
   </si>
 </sst>
 </file>
@@ -438,7 +447,7 @@
   <sheetData>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" x14ac:dyDescent="0.35">
       <c r="A1" s="0" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>2</v>
@@ -452,10 +461,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="0">
-        <v>80.680000000000007</v>
+        <v>78.849999999999994</v>
       </c>
       <c r="C2" s="0">
-        <v>19.079999999999998</v>
+        <v>16.600000000000001</v>
       </c>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.35">
@@ -463,10 +472,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="0">
-        <v>81.909999999999997</v>
+        <v>79.790000000000006</v>
       </c>
       <c r="C3" s="0">
-        <v>39.229999999999997</v>
+        <v>36.450000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>